<commit_message>
Rev 3 of Gage R&R report
</commit_message>
<xml_diff>
--- a/_4 Validation/QA Gage R&R/$MLOI_CalRecord v3.xlsx
+++ b/_4 Validation/QA Gage R&R/$MLOI_CalRecord v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllenProjects\PM_Folder\_4 Validation\QA Gage R&amp;R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC6B04A-21E6-4599-80EC-83309CDB4019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BC11B6-6E4B-464E-965D-B026822558B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="3750" windowWidth="19125" windowHeight="14040" activeTab="2" xr2:uid="{E8277EBF-8E94-4486-9664-CBE43E0BB732}"/>
+    <workbookView xWindow="3555" yWindow="1545" windowWidth="21600" windowHeight="11715" activeTab="3" xr2:uid="{E8277EBF-8E94-4486-9664-CBE43E0BB732}"/>
   </bookViews>
   <sheets>
     <sheet name="Elevate Level" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="137">
   <si>
     <t>Index</t>
   </si>
@@ -649,6 +649,15 @@
       <t>W</t>
     </r>
   </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Cal Date</t>
+  </si>
+  <si>
+    <t>Calibrator</t>
+  </si>
 </sst>
 </file>
 
@@ -665,7 +674,7 @@
     <numFmt numFmtId="171" formatCode="0.00000"/>
     <numFmt numFmtId="172" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,6 +802,26 @@
       <name val="Symbol"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1055,7 +1084,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1198,62 +1227,242 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="17" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="17" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="94">
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2164,6 +2373,57 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -5861,14 +6121,14 @@
               <c:f>'Resistance ChB R&amp;R'!$I$2:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
                   <c:v>1.2000000000000455E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.6999999999995907E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2.8999999999996362E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -5909,14 +6169,14 @@
               <c:f>'Resistance ChB R&amp;R'!$J$2:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
                   <c:v>4.3333333333333002E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3.4333333333333327E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3.8666666666666627E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -8198,40 +8458,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4.166666666667318E-4</c:v>
+                  <c:v>9.0909090909141455E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.166666666667318E-4</c:v>
+                  <c:v>9.0909090909141455E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4166666666667327E-3</c:v>
+                  <c:v>1.0909090909091423E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.166666666667318E-4</c:v>
+                  <c:v>9.0909090909141455E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.166666666667318E-4</c:v>
+                  <c:v>9.0909090909141455E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.166666666667318E-4</c:v>
+                  <c:v>9.0909090909141455E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.166666666667318E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5833333333332718E-3</c:v>
+                  <c:v>9.0909090909141455E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.166666666667318E-4</c:v>
+                  <c:v>9.0909090909141455E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.58333333333327E-3</c:v>
+                  <c:v>1.9090909090908603E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.8333333333326909E-4</c:v>
+                  <c:v>9.0909090909085943E-4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4166666666667327E-3</c:v>
+                  <c:v>1.0909090909091423E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8273,40 +8530,37 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.4999999999995026E-3</c:v>
+                  <c:v>1.6363636363632139E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5000000000000568E-3</c:v>
+                  <c:v>6.3636363636376814E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4999999999991758E-3</c:v>
+                  <c:v>8.6363636363628871E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4999999999995026E-3</c:v>
+                  <c:v>1.6363636363632139E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.500000000001279E-3</c:v>
+                  <c:v>3.3636363636375677E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.500000000001279E-3</c:v>
+                  <c:v>3.3636363636375677E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0000000000061107E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.5000000000009521E-3</c:v>
+                  <c:v>1.3636363636368998E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4999999999989484E-3</c:v>
+                  <c:v>2.6363636363626597E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.5000000000008384E-3</c:v>
+                  <c:v>7.3636363636371271E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5000000000000568E-3</c:v>
+                  <c:v>2.3636363636363455E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.4999999999989484E-3</c:v>
+                  <c:v>2.6363636363626597E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16354,15 +16608,15 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16980,21 +17234,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36D874EF-83D9-4578-ADA6-780A68E381AC}" name="Table1" displayName="Table1" ref="A1:J13" totalsRowShown="0" headerRowDxfId="75" headerRowBorderDxfId="74" tableBorderDxfId="73" totalsRowBorderDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{36D874EF-83D9-4578-ADA6-780A68E381AC}" name="Table1" displayName="Table1" ref="A1:J13" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
   <autoFilter ref="A1:J13" xr:uid="{36D874EF-83D9-4578-ADA6-780A68E381AC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F2721F03-CD74-4299-9934-A97CA5605160}" name="CAL ID" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{82E82C70-B493-4814-B426-9F482770C84C}" name="Operator" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{17A80109-5FCF-423D-B8B1-46156C5CAE44}" name="Date/Time" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{37901583-2E3D-497B-BB57-C01CCDA835B9}" name="OP" dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{7CF7A247-90CB-4603-8A3C-8BDD90341B3B}" name="Trial" dataDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{074E1160-B8F3-4818-B95B-B30B6EB2C33F}" name="Goodness" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{ACA87EA0-C87C-4BA1-93F1-1A292C39F7F0}" name="Slope" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{5659EEDD-9BC3-4597-B2FA-1CFF391D941B}" name="Intercept" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{648B25B4-1EA1-4103-8B0C-02F9E4E8212A}" name="Slope Dev" dataDxfId="66">
+    <tableColumn id="1" xr3:uid="{F2721F03-CD74-4299-9934-A97CA5605160}" name="CAL ID" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{82E82C70-B493-4814-B426-9F482770C84C}" name="Operator" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{17A80109-5FCF-423D-B8B1-46156C5CAE44}" name="Date/Time" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{37901583-2E3D-497B-BB57-C01CCDA835B9}" name="OP" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{7CF7A247-90CB-4603-8A3C-8BDD90341B3B}" name="Trial" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{074E1160-B8F3-4818-B95B-B30B6EB2C33F}" name="Goodness" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{ACA87EA0-C87C-4BA1-93F1-1A292C39F7F0}" name="Slope" dataDxfId="83"/>
+    <tableColumn id="8" xr3:uid="{5659EEDD-9BC3-4597-B2FA-1CFF391D941B}" name="Intercept" dataDxfId="82"/>
+    <tableColumn id="9" xr3:uid="{648B25B4-1EA1-4103-8B0C-02F9E4E8212A}" name="Slope Dev" dataDxfId="81">
       <calculatedColumnFormula>ABS(Table1[[#This Row],[Slope]]-$P$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A9701F3C-D887-4A06-BCBB-22C3CA97C5A5}" name="Int Dev" dataDxfId="65">
+    <tableColumn id="10" xr3:uid="{A9701F3C-D887-4A06-BCBB-22C3CA97C5A5}" name="Int Dev" dataDxfId="80">
       <calculatedColumnFormula>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -17008,55 +17262,55 @@
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{E357F212-1130-467F-A35D-F7A996DE25AB}" name="Run ID"/>
     <tableColumn id="2" xr3:uid="{8CBE0BDF-FD1F-459A-884F-CF8D5B16B006}" name="Operator"/>
-    <tableColumn id="3" xr3:uid="{57E7B8AF-7C91-49AC-A6C4-80E90EC8426A}" name="Date/Time" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{57E7B8AF-7C91-49AC-A6C4-80E90EC8426A}" name="Date/Time" dataDxfId="79"/>
     <tableColumn id="4" xr3:uid="{6D239A18-3677-4B0E-8CB6-D21D806EC8F5}" name="Op"/>
     <tableColumn id="5" xr3:uid="{7F9984A8-8CA3-48DA-950D-741DA5450FBC}" name="Trial"/>
     <tableColumn id="6" xr3:uid="{6F2B7BB7-D43C-4A46-A942-6CF43774305D}" name="Set Point"/>
-    <tableColumn id="7" xr3:uid="{F5C7061A-2C5A-4683-8CAD-78DFFB9ADB70}" name="Set Point2" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{09199FD2-A1C0-4BFE-AEF9-9B86C713A6E5}" name="Op * Laser" dataDxfId="62">
+    <tableColumn id="7" xr3:uid="{F5C7061A-2C5A-4683-8CAD-78DFFB9ADB70}" name="Set Point2" dataDxfId="78"/>
+    <tableColumn id="11" xr3:uid="{09199FD2-A1C0-4BFE-AEF9-9B86C713A6E5}" name="Op * Laser" dataDxfId="77">
       <calculatedColumnFormula>Table4[[#This Row],[Op]]*Table4[[#This Row],[Laser^2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E506D6F6-5C86-471C-86BE-F0677880E48A}" name="Laser^2" dataDxfId="61">
+    <tableColumn id="10" xr3:uid="{E506D6F6-5C86-471C-86BE-F0677880E48A}" name="Laser^2" dataDxfId="76">
       <calculatedColumnFormula>Table4[[#This Row],[Laser]]^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6F033725-5949-4E6B-845C-A295270B9256}" name="OP(2)" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{C4E8308E-5DE2-41C0-962D-DD8992DAE6D8}" name="Laser" dataDxfId="59"/>
-    <tableColumn id="9" xr3:uid="{B1288E4D-EB2C-415E-B70B-F4983B4EF68E}" name="Measure" dataDxfId="58"/>
-    <tableColumn id="28" xr3:uid="{BB6A6514-0BA8-4D00-ACBB-6EF40A4B2381}" name="Column14" dataDxfId="57"/>
-    <tableColumn id="14" xr3:uid="{99B6E85A-410A-4A2A-AEE3-F06EFBEA7A07}" name="Column1" dataDxfId="56"/>
-    <tableColumn id="15" xr3:uid="{C778E956-8BE5-430D-978D-BC020F6A644E}" name="Column2" dataDxfId="55"/>
-    <tableColumn id="16" xr3:uid="{680FF82D-ED70-48EB-8400-F81966ECFB63}" name="Column3" dataDxfId="54"/>
-    <tableColumn id="17" xr3:uid="{93B9B5E0-75A1-48CA-AA5B-F80D14FC663F}" name="Column4" dataDxfId="53"/>
-    <tableColumn id="18" xr3:uid="{10FF20CC-1780-44AC-8429-3902FA89087F}" name="Column5" dataDxfId="52"/>
-    <tableColumn id="19" xr3:uid="{D224446E-94C9-471A-8AA1-E2384C2B57A0}" name="Column6" dataDxfId="51"/>
-    <tableColumn id="20" xr3:uid="{1F80C397-7C4B-4E4F-BC5A-49F8EBB37A29}" name="Column7" dataDxfId="50"/>
-    <tableColumn id="21" xr3:uid="{05D840E5-C046-4567-88BB-CBC5854A0B27}" name="Column8" dataDxfId="49"/>
-    <tableColumn id="22" xr3:uid="{F864F628-3FAA-4474-B999-BB4DD0D8443D}" name="Column9" dataDxfId="48"/>
-    <tableColumn id="23" xr3:uid="{510EEA27-3978-4F79-9391-86C4AD5A1DF3}" name="Column10" dataDxfId="47"/>
-    <tableColumn id="24" xr3:uid="{02B4D1BD-B6C6-4CDC-9158-533F313AAF6F}" name="Column11" dataDxfId="46"/>
-    <tableColumn id="25" xr3:uid="{65DC09A2-59F1-494A-97C2-41EB80847CDE}" name="Column12" dataDxfId="45"/>
-    <tableColumn id="26" xr3:uid="{A3D1B302-20BB-49FE-947E-D6D3356BA7EC}" name="Column13" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{6F033725-5949-4E6B-845C-A295270B9256}" name="OP(2)" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{C4E8308E-5DE2-41C0-962D-DD8992DAE6D8}" name="Laser" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{B1288E4D-EB2C-415E-B70B-F4983B4EF68E}" name="Measure" dataDxfId="73"/>
+    <tableColumn id="28" xr3:uid="{BB6A6514-0BA8-4D00-ACBB-6EF40A4B2381}" name="Column14" dataDxfId="72"/>
+    <tableColumn id="14" xr3:uid="{99B6E85A-410A-4A2A-AEE3-F06EFBEA7A07}" name="Column1" dataDxfId="71"/>
+    <tableColumn id="15" xr3:uid="{C778E956-8BE5-430D-978D-BC020F6A644E}" name="Column2" dataDxfId="70"/>
+    <tableColumn id="16" xr3:uid="{680FF82D-ED70-48EB-8400-F81966ECFB63}" name="Column3" dataDxfId="69"/>
+    <tableColumn id="17" xr3:uid="{93B9B5E0-75A1-48CA-AA5B-F80D14FC663F}" name="Column4" dataDxfId="68"/>
+    <tableColumn id="18" xr3:uid="{10FF20CC-1780-44AC-8429-3902FA89087F}" name="Column5" dataDxfId="67"/>
+    <tableColumn id="19" xr3:uid="{D224446E-94C9-471A-8AA1-E2384C2B57A0}" name="Column6" dataDxfId="66"/>
+    <tableColumn id="20" xr3:uid="{1F80C397-7C4B-4E4F-BC5A-49F8EBB37A29}" name="Column7" dataDxfId="65"/>
+    <tableColumn id="21" xr3:uid="{05D840E5-C046-4567-88BB-CBC5854A0B27}" name="Column8" dataDxfId="64"/>
+    <tableColumn id="22" xr3:uid="{F864F628-3FAA-4474-B999-BB4DD0D8443D}" name="Column9" dataDxfId="63"/>
+    <tableColumn id="23" xr3:uid="{510EEA27-3978-4F79-9391-86C4AD5A1DF3}" name="Column10" dataDxfId="62"/>
+    <tableColumn id="24" xr3:uid="{02B4D1BD-B6C6-4CDC-9158-533F313AAF6F}" name="Column11" dataDxfId="61"/>
+    <tableColumn id="25" xr3:uid="{65DC09A2-59F1-494A-97C2-41EB80847CDE}" name="Column12" dataDxfId="60"/>
+    <tableColumn id="26" xr3:uid="{A3D1B302-20BB-49FE-947E-D6D3356BA7EC}" name="Column13" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{81D4D0B3-8575-433B-A8F1-8A4D99C086DD}" name="Table16" displayName="Table16" ref="A1:J5" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{81D4D0B3-8575-433B-A8F1-8A4D99C086DD}" name="Table16" displayName="Table16" ref="A1:J5" totalsRowShown="0" headerRowDxfId="58">
   <autoFilter ref="A1:J5" xr:uid="{36D874EF-83D9-4578-ADA6-780A68E381AC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{748AF1BC-CC4F-4DE4-962E-47A4B6005190}" name="CAL ID" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{43FDE7C9-F46F-4492-9EA1-0C87DBED3250}" name="Operator" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{DAE0DEE9-625B-4277-A75B-9DD85D2CC808}" name="Date/Time" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{26017869-FCA2-49A1-B10D-1237E22B6E41}" name="OP" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{B692C333-02A3-4F2B-92FA-CF0271950F18}" name="Trial" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{0A612A20-9D0C-4797-A149-C34AC5F0448C}" name="Channel" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{137390AD-9DC3-4A0D-A5AF-0225BAD06578}" name="Slope" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{FDBF0999-6CFE-4421-B7F9-1A6B03783DE6}" name="Intercept" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{C7A592F7-AC00-4089-B6FD-28A373ADE946}" name="Slope Dev" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{748AF1BC-CC4F-4DE4-962E-47A4B6005190}" name="CAL ID" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{43FDE7C9-F46F-4492-9EA1-0C87DBED3250}" name="Operator" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{DAE0DEE9-625B-4277-A75B-9DD85D2CC808}" name="Date/Time" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{26017869-FCA2-49A1-B10D-1237E22B6E41}" name="OP" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{B692C333-02A3-4F2B-92FA-CF0271950F18}" name="Trial" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{0A612A20-9D0C-4797-A149-C34AC5F0448C}" name="Channel" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{137390AD-9DC3-4A0D-A5AF-0225BAD06578}" name="Slope" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{FDBF0999-6CFE-4421-B7F9-1A6B03783DE6}" name="Intercept" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{C7A592F7-AC00-4089-B6FD-28A373ADE946}" name="Slope Dev" dataDxfId="49">
       <calculatedColumnFormula>ABS(Table16[[#This Row],[Slope]]-$N$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{857F8E7A-CE96-4142-BA0E-44FD74485E68}" name="Int Dev" dataDxfId="33">
+    <tableColumn id="10" xr3:uid="{857F8E7A-CE96-4142-BA0E-44FD74485E68}" name="Int Dev" dataDxfId="48">
       <calculatedColumnFormula>ABS(Table16[[#This Row],[Intercept]]-$O$7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -17065,21 +17319,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0AD647EE-AC7A-401F-A5A8-C967E193F1CA}" name="Table163" displayName="Table163" ref="A18:J24" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0AD647EE-AC7A-401F-A5A8-C967E193F1CA}" name="Table163" displayName="Table163" ref="A18:J24" totalsRowShown="0" headerRowDxfId="47">
   <autoFilter ref="A18:J24" xr:uid="{0AD647EE-AC7A-401F-A5A8-C967E193F1CA}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{0B5C75E3-D268-4C1B-A84E-5BE68FD2C4A6}" name="CAL ID" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{34B28A9A-3E1F-4944-97CB-642C93A48C87}" name="Operator" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{1B94585A-EDAC-4DAD-9B02-5EE26787484D}" name="Date/Time" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{9F1223F8-2F08-4C80-8436-E66B30404C38}" name="OP" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{7176B3AA-04AD-408B-97AD-033C927FB8EC}" name="Trial" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{4076CFBD-9D1A-4DB5-B44E-69F81169D4D1}" name="Channel" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{82CBCA22-9DC2-42D7-B863-E23C9F1E851F}" name="Slope" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{124F70CE-D8D1-4C15-81B1-BFEF25BA4A72}" name="Intercept" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{B403DA03-FFE2-445A-92CC-0A94240E1EE7}" name="Slope Dev" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{0B5C75E3-D268-4C1B-A84E-5BE68FD2C4A6}" name="CAL ID" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{34B28A9A-3E1F-4944-97CB-642C93A48C87}" name="Operator" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{1B94585A-EDAC-4DAD-9B02-5EE26787484D}" name="Date/Time" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{9F1223F8-2F08-4C80-8436-E66B30404C38}" name="OP" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{7176B3AA-04AD-408B-97AD-033C927FB8EC}" name="Trial" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{4076CFBD-9D1A-4DB5-B44E-69F81169D4D1}" name="Channel" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{82CBCA22-9DC2-42D7-B863-E23C9F1E851F}" name="Slope" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{124F70CE-D8D1-4C15-81B1-BFEF25BA4A72}" name="Intercept" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{B403DA03-FFE2-445A-92CC-0A94240E1EE7}" name="Slope Dev" dataDxfId="38">
       <calculatedColumnFormula>ABS(Table168[[#This Row],[Slope]]-$N$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A0F621B6-2E07-4AC4-8A3D-309DF0B7CF82}" name="Int Dev" dataDxfId="22">
+    <tableColumn id="10" xr3:uid="{A0F621B6-2E07-4AC4-8A3D-309DF0B7CF82}" name="Int Dev" dataDxfId="37">
       <calculatedColumnFormula>ABS(Table168[[#This Row],[Intercept]]-$O$7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -17088,21 +17342,21 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3BEB4358-1238-4D9D-8909-1E959DBB847D}" name="Table168" displayName="Table168" ref="A1:J5" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3BEB4358-1238-4D9D-8909-1E959DBB847D}" name="Table168" displayName="Table168" ref="A1:J5" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:J5" xr:uid="{36D874EF-83D9-4578-ADA6-780A68E381AC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{093175AC-6E59-45ED-A43D-3CBFF671CE19}" name="CAL ID" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{0955E3AF-324C-4B8D-BB11-5361CB097A2D}" name="Operator" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{E7A8D6B8-6A38-46BF-AD04-DA50631B1FE6}" name="Date/Time" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{55A3479B-0634-4800-803A-E6E508211B06}" name="OP" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{7343A4B7-DB13-472B-889A-DFED38F7F37F}" name="Trial" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{A33511BD-9E55-4845-ABFA-4BB044A1A540}" name="Channel" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{C2039754-7142-44EE-A09B-E9768EA31EF8}" name="Slope" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{A98267E6-3ACD-44E7-B07E-79AAA4D69EF8}" name="Intercept" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{801CE742-1ED2-4742-B148-BA4115ADE492}" name="Slope Dev" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{093175AC-6E59-45ED-A43D-3CBFF671CE19}" name="CAL ID" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{0955E3AF-324C-4B8D-BB11-5361CB097A2D}" name="Operator" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{E7A8D6B8-6A38-46BF-AD04-DA50631B1FE6}" name="Date/Time" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{55A3479B-0634-4800-803A-E6E508211B06}" name="OP" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{7343A4B7-DB13-472B-889A-DFED38F7F37F}" name="Trial" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{A33511BD-9E55-4845-ABFA-4BB044A1A540}" name="Channel" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{C2039754-7142-44EE-A09B-E9768EA31EF8}" name="Slope" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{A98267E6-3ACD-44E7-B07E-79AAA4D69EF8}" name="Intercept" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{801CE742-1ED2-4742-B148-BA4115ADE492}" name="Slope Dev" dataDxfId="27">
       <calculatedColumnFormula>ABS(Table168[[#This Row],[Slope]]-$N$7)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{565ADF9B-A304-49C3-A18E-26E9C384A956}" name="Int Dev" dataDxfId="11">
+    <tableColumn id="10" xr3:uid="{565ADF9B-A304-49C3-A18E-26E9C384A956}" name="Int Dev" dataDxfId="26">
       <calculatedColumnFormula>ABS(Table168[[#This Row],[Intercept]]-$O$7)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -22232,7 +22486,7 @@
   <dimension ref="A2:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A9" sqref="A9:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22359,7 +22613,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5">
         <v>45784.392361111109</v>
@@ -22691,8 +22945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED8B73E-9C03-4CC9-A7A6-29D3E7915FAA}">
   <dimension ref="A1:AE167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G13"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22710,13 +22964,15 @@
     <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.140625" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" customWidth="1"/>
     <col min="30" max="30" width="10.42578125" customWidth="1"/>
     <col min="31" max="31" width="11" customWidth="1"/>
     <col min="32" max="32" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>53</v>
       </c>
@@ -22761,7 +23017,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="43">
         <v>1</v>
       </c>
@@ -22788,11 +23044,11 @@
       </c>
       <c r="I2" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>4.166666666667318E-4</v>
+        <v>9.0909090909141455E-5</v>
       </c>
       <c r="J2" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>2.4999999999995026E-3</v>
+        <v>1.6363636363632139E-3</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -22803,7 +23059,7 @@
       </c>
       <c r="P2" s="15">
         <f>COUNTA(Table1[CAL ID])</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S2" s="65">
         <v>0.9</v>
@@ -22816,7 +23072,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="43">
         <v>2</v>
       </c>
@@ -22843,11 +23099,11 @@
       </c>
       <c r="I3" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>4.166666666667318E-4</v>
+        <v>9.0909090909141455E-5</v>
       </c>
       <c r="J3" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>1.5000000000000568E-3</v>
+        <v>6.3636363636376814E-4</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -22866,7 +23122,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="43">
         <v>3</v>
       </c>
@@ -22893,11 +23149,11 @@
       </c>
       <c r="I4" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>1.4166666666667327E-3</v>
+        <v>1.0909090909091423E-3</v>
       </c>
       <c r="J4" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>9.4999999999991758E-3</v>
+        <v>8.6363636363628871E-3</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -22916,7 +23172,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="43">
         <v>4</v>
       </c>
@@ -22943,18 +23199,33 @@
       </c>
       <c r="I5" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>4.166666666667318E-4</v>
+        <v>9.0909090909141455E-5</v>
       </c>
       <c r="J5" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>2.4999999999995026E-3</v>
+        <v>1.6363636363632139E-3</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y5" s="84" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z5" s="85" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA5" s="86" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB5" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC5" s="87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="43">
         <v>5</v>
       </c>
@@ -22981,11 +23252,11 @@
       </c>
       <c r="I6" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>4.166666666667318E-4</v>
+        <v>9.0909090909141455E-5</v>
       </c>
       <c r="J6" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>2.500000000001279E-3</v>
+        <v>3.3636363636375677E-3</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="18" t="s">
@@ -23015,8 +23286,23 @@
       <c r="W6" s="69" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y6" s="88" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z6" s="89">
+        <v>45689</v>
+      </c>
+      <c r="AA6" s="89" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB6" s="90">
+        <v>-0.99650000000000005</v>
+      </c>
+      <c r="AC6" s="90">
+        <v>9.5974000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="43">
         <v>6</v>
       </c>
@@ -23043,11 +23329,11 @@
       </c>
       <c r="I7" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>4.166666666667318E-4</v>
+        <v>9.0909090909141455E-5</v>
       </c>
       <c r="J7" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>2.500000000001279E-3</v>
+        <v>3.3636363636375677E-3</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -23058,34 +23344,48 @@
       </c>
       <c r="P7" s="15" cm="1">
         <f t="array" ref="P7">AVERAGE(IF(Table1[OP]&lt;&gt;O6,Table1[Slope],""))</f>
-        <v>-0.99658333333333327</v>
+        <v>-0.99690909090909086</v>
       </c>
       <c r="Q7" s="15" cm="1">
         <f t="array" ref="Q7">AVERAGE(IF(Table1[OP]&lt;&gt;O6,Table1[Intercept],""))</f>
-        <v>9.5965000000000007</v>
+        <v>9.597363636363637</v>
       </c>
       <c r="S7" s="15">
         <v>8.4</v>
       </c>
       <c r="T7" s="15">
         <f ca="1">$P$9*S7</f>
-        <v>-8.379926969530068</v>
+        <v>-8.3794677800828232</v>
       </c>
       <c r="U7" s="15">
         <f ca="1">S7*$P$10</f>
-        <v>-8.3626730304699315</v>
+        <v>-8.3686049471899029</v>
       </c>
       <c r="V7" s="16">
         <f ca="1">T7-U7</f>
-        <v>-1.7253939060136503E-2</v>
+        <v>-1.0862832892920338E-2</v>
       </c>
       <c r="W7" s="40">
         <f ca="1">ABS(V7/2)</f>
-        <v>8.6269695300682514E-3</v>
-      </c>
-      <c r="Y7" s="70"/>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5.4314164464601689E-3</v>
+      </c>
+      <c r="Y7" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="89">
+        <v>45317</v>
+      </c>
+      <c r="AA7" s="89" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB7" s="90">
+        <v>112.468</v>
+      </c>
+      <c r="AC7" s="90">
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="43">
         <v>7</v>
       </c>
@@ -23112,11 +23412,11 @@
       </c>
       <c r="I8" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>4.166666666667318E-4</v>
+        <v>9.0909090909141455E-5</v>
       </c>
       <c r="J8" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>5.0000000000061107E-4</v>
+        <v>1.3636363636368998E-3</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
@@ -23129,65 +23429,58 @@
       </c>
       <c r="P8" s="15" cm="1">
         <f t="array" ref="P8">_xlfn.STDEV.S(IF(Table1[OP]&lt;&gt;O6,Table1[Slope],""))</f>
-        <v>1.3789543689024502E-3</v>
+        <v>8.3120941459363423E-4</v>
       </c>
       <c r="Q8" s="15" cm="1">
         <f t="array" ref="Q8">_xlfn.STDEV.S(IF(Table1[OP]&lt;&gt;O6,Table1[Intercept],""))</f>
-        <v>5.0181488799973693E-3</v>
+        <v>4.2254639336463109E-3</v>
       </c>
       <c r="S8" s="15">
         <v>2.75</v>
       </c>
       <c r="T8" s="15">
         <f ca="1">$P$9*S8</f>
-        <v>-2.7434284721675817</v>
+        <v>-2.7432781422890193</v>
       </c>
       <c r="U8" s="15">
         <f ca="1">S8*$P$10</f>
-        <v>-2.7377798611657513</v>
+        <v>-2.7397218577109803</v>
       </c>
       <c r="V8" s="16">
         <f ca="1">T8-U8</f>
-        <v>-5.6486110018303393E-3</v>
+        <v>-3.5562845780390262E-3</v>
       </c>
       <c r="W8" s="40">
         <f ca="1">ABS(V8/2)</f>
-        <v>2.8243055009151696E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <v>8</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="45">
-        <v>45796.415277777778</v>
-      </c>
-      <c r="D9" s="15">
-        <v>3</v>
-      </c>
-      <c r="E9" s="15">
-        <v>2</v>
-      </c>
-      <c r="F9" s="20">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G9" s="40">
-        <v>-0.99299999999999999</v>
-      </c>
-      <c r="H9" s="20">
-        <v>9.5869999999999997</v>
-      </c>
-      <c r="I9" s="20">
-        <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>3.5833333333332718E-3</v>
-      </c>
-      <c r="J9" s="20">
-        <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>9.5000000000009521E-3</v>
-      </c>
+        <v>1.7781422890195131E-3</v>
+      </c>
+      <c r="Y8" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="89">
+        <v>45317</v>
+      </c>
+      <c r="AA8" s="89" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB8" s="90">
+        <v>113.95</v>
+      </c>
+      <c r="AC8" s="90">
+        <v>-1.236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="46"/>
       <c r="K9" s="3"/>
       <c r="L9" s="19">
         <v>0.99</v>
@@ -23199,14 +23492,14 @@
       </c>
       <c r="P9" s="40">
         <f ca="1">P$7-$U$2*P$8/$P$2^0.5</f>
-        <v>-0.99761035351548422</v>
+        <v>-0.99755568810509798</v>
       </c>
       <c r="Q9" s="40">
         <f ca="1">Q$7-$U$2*Q$8/$P$2^0.5</f>
-        <v>9.5927625738073576</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+        <v>9.5940766510584226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="43">
         <v>9</v>
       </c>
@@ -23233,11 +23526,11 @@
       </c>
       <c r="I10" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>4.166666666667318E-4</v>
+        <v>9.0909090909141455E-5</v>
       </c>
       <c r="J10" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>3.4999999999989484E-3</v>
+        <v>2.6363636363626597E-3</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -23248,21 +23541,21 @@
       </c>
       <c r="P10" s="40">
         <f ca="1">P$7+$U$2*P$8/$P$2^0.5</f>
-        <v>-0.99555631315118231</v>
+        <v>-0.99626249371308373</v>
       </c>
       <c r="Q10" s="40">
         <f ca="1">Q$7+U$2*Q$8/$P$2^0.5</f>
-        <v>9.6002374261926438</v>
+        <v>9.6006506216688514</v>
       </c>
       <c r="V10" s="67" t="s">
         <v>130</v>
       </c>
       <c r="W10" s="68" t="str">
         <f ca="1">"±" &amp; ROUND(MAX(W7/S7,W8/S8)*100,3) &amp; "%"</f>
-        <v>±0.103%</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+        <v>±0.065%</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="43">
         <v>10</v>
       </c>
@@ -23289,18 +23582,18 @@
       </c>
       <c r="I11" s="20">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>1.58333333333327E-3</v>
+        <v>1.9090909090908603E-3</v>
       </c>
       <c r="J11" s="46">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>6.5000000000008384E-3</v>
+        <v>7.3636363636371271E-3</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="47">
         <v>11</v>
       </c>
@@ -23327,18 +23620,18 @@
       </c>
       <c r="I12" s="50">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>5.8333333333326909E-4</v>
+        <v>9.0909090909085943E-4</v>
       </c>
       <c r="J12" s="51">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>1.5000000000000568E-3</v>
+        <v>2.3636363636363455E-3</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52">
         <v>12</v>
       </c>
@@ -23365,16 +23658,50 @@
       </c>
       <c r="I13" s="56">
         <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
-        <v>1.4166666666667327E-3</v>
+        <v>1.0909090909091423E-3</v>
       </c>
       <c r="J13" s="57">
         <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
-        <v>3.4999999999989484E-3</v>
+        <v>2.6363636363626597E-3</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>8</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="45">
+        <v>45796.415277777778</v>
+      </c>
+      <c r="D16" s="15">
+        <v>3</v>
+      </c>
+      <c r="E16" s="15">
+        <v>2</v>
+      </c>
+      <c r="F16" s="20">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G16" s="40">
+        <v>-0.99299999999999999</v>
+      </c>
+      <c r="H16" s="20">
+        <v>9.5869999999999997</v>
+      </c>
+      <c r="I16" s="20" t="e">
+        <f>ABS(Table1[[#This Row],[Slope]]-$P$7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J16" s="20" t="e">
+        <f>ABS(Table1[[#This Row],[Intercept]]-$Q$7)</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K17" s="3"/>
@@ -29189,14 +29516,22 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="I2:I13">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="I2:I8 I10:I13 I16">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
       <formula>0.002</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="J2:J8 J10:J13 J16">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="greaterThan">
       <formula>0.006</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB5:AC8">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -29218,8 +29553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23445DBE-5D88-41CB-B169-526E1B5623C8}">
   <dimension ref="A1:W75"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:V10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29597,11 +29932,19 @@
         <f ca="1">MAX(W7/Q7,W8/Q8)</f>
         <v>1.1363691461062759E-3</v>
       </c>
+      <c r="W10" s="70">
+        <f ca="1">1-S7/Q7</f>
+        <v>1.1363691461062642E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
+      <c r="W11" s="70">
+        <f ca="1">1-T8/Q8</f>
+        <v>-2.6168473902221656E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D12" s="6" t="s">
@@ -30172,22 +30515,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I5 I19:J21">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:I24">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J5">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J24">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30211,7 +30554,7 @@
   <dimension ref="A1:W76"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="M6" sqref="M6:V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30267,7 +30610,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="1"/>
       <c r="C2" s="5"/>
@@ -30589,6 +30932,7 @@
         <f ca="1">MAX(W7/Q7,W8/Q8)</f>
         <v>2.2890038109144436E-3</v>
       </c>
+      <c r="W10" s="70"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="J11" s="3"/>
@@ -30981,12 +31325,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I5">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>